<commit_message>
#14 Updated todo page feature test cases and test outputs
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDo.xlsx
+++ b/TestCases/Test Cases - ToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI CA1.2\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65483EB-8E66-4661-9C0B-B4347BF90D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BCDAB-84D0-4876-B6F1-2537DE915F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Fail/Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>-</t>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>The user will be brought to the to-do page.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
   </si>
 </sst>
 </file>
@@ -478,24 +481,24 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -516,122 +519,122 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2.1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2.2999999999999998</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2.4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -640,7 +643,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -649,7 +652,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -658,7 +661,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -667,7 +670,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -676,7 +679,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -685,7 +688,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -694,7 +697,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -703,7 +706,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>

</xml_diff>

<commit_message>
Added Registration test cases, Updated ToDo page test cases documentation
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDo.xlsx
+++ b/TestCases/Test Cases - ToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BCDAB-84D0-4876-B6F1-2537DE915F0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB857569-EBE4-4DB2-9E64-ED61388B76AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Test deleting a to-do item</t>
   </si>
   <si>
-    <t>Test archiving a to-do item</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -108,6 +105,39 @@
   </si>
   <si>
     <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test successful display of to-do items based on user</t>
+  </si>
+  <si>
+    <t>To check if to-do items can only be seen by the user that has created it.</t>
+  </si>
+  <si>
+    <t>The to-do items that are unique to the user will be shown successfully.</t>
+  </si>
+  <si>
+    <t>The to-do items with timestamps will be shown successfully.</t>
+  </si>
+  <si>
+    <t>Test automatically archiving after completing a to-do item</t>
+  </si>
+  <si>
+    <t>To check if to-do items have individual timestamps of creation datetime.</t>
+  </si>
+  <si>
+    <t>Test displaying of timestamp (creation date) of to-do item</t>
+  </si>
+  <si>
+    <t>Test displaying of individual to-do items for each user</t>
+  </si>
+  <si>
+    <t>To test if the to-do items shown are the ones created by the user and not other users.</t>
+  </si>
+  <si>
+    <t>After user log in, he/she sees only his/her own to-do items. Logging into another user's account will show a different list of to-do items.</t>
   </si>
 </sst>
 </file>
@@ -480,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +528,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -524,22 +554,22 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -550,19 +580,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -573,19 +603,19 @@
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,22 +623,22 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -619,57 +649,91 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
+      <c r="A8" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>

</xml_diff>

<commit_message>
Removal of duplicated test case from todo test case documentation
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDo.xlsx
+++ b/TestCases/Test Cases - ToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\test todo list\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB857569-EBE4-4DB2-9E64-ED61388B76AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425908A9-E00C-49EA-8563-21080528B8C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -108,15 +108,6 @@
   </si>
   <si>
     <t>Fail</t>
-  </si>
-  <si>
-    <t>Test successful display of to-do items based on user</t>
-  </si>
-  <si>
-    <t>To check if to-do items can only be seen by the user that has created it.</t>
-  </si>
-  <si>
-    <t>The to-do items that are unique to the user will be shown successfully.</t>
   </si>
   <si>
     <t>The to-do items with timestamps will be shown successfully.</t>
@@ -511,7 +502,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +614,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>16</v>
@@ -669,16 +660,16 @@
         <v>2.5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>6</v>
@@ -692,7 +683,7 @@
         <v>2.6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>32</v>
@@ -701,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>6</v>
@@ -710,29 +701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="9" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>

</xml_diff>

<commit_message>
#23 Updated/Added new test cases for to-do page features
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDo.xlsx
+++ b/TestCases/Test Cases - ToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\test todo list\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425908A9-E00C-49EA-8563-21080528B8C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F9DC79-C2A7-4E23-AC32-7376E9AF2FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>After user log in, he/she sees only his/her own to-do items. Logging into another user's account will show a different list of to-do items.</t>
+  </si>
+  <si>
+    <t>Item cannot be automatically archived.</t>
+  </si>
+  <si>
+    <t>Item cannot be deleted.</t>
+  </si>
+  <si>
+    <t>Timestamp is not being displayed.</t>
+  </si>
+  <si>
+    <t>The to-do items are not filtered by users. All users see the same set of to-do items.</t>
   </si>
 </sst>
 </file>
@@ -501,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,10 +615,10 @@
         <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -626,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>26</v>
@@ -672,7 +684,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>26</v>
@@ -695,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
#25 Updated test outputs pictures and test cases documentation
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDo.xlsx
+++ b/TestCases/Test Cases - ToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\ETI-ToDoList (GitHub)\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\test todo list 2\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F9DC79-C2A7-4E23-AC32-7376E9AF2FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8551AB2E-DE86-4089-B892-74242AF36148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Same as expected outcome.</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>The to-do items with timestamps will be shown successfully.</t>
   </si>
   <si>
@@ -129,18 +126,6 @@
   </si>
   <si>
     <t>After user log in, he/she sees only his/her own to-do items. Logging into another user's account will show a different list of to-do items.</t>
-  </si>
-  <si>
-    <t>Item cannot be automatically archived.</t>
-  </si>
-  <si>
-    <t>Item cannot be deleted.</t>
-  </si>
-  <si>
-    <t>Timestamp is not being displayed.</t>
-  </si>
-  <si>
-    <t>The to-do items are not filtered by users. All users see the same set of to-do items.</t>
   </si>
 </sst>
 </file>
@@ -513,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,10 +600,10 @@
         <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -626,7 +611,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>16</v>
@@ -638,10 +623,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -672,22 +657,22 @@
         <v>2.5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -695,22 +680,22 @@
         <v>2.6</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>